<commit_message>
1020 ALTER PPT # Please enter the commit message for your changes. Lines      starting
</commit_message>
<xml_diff>
--- a/快递管理系统/课堂记录.xlsx
+++ b/快递管理系统/课堂记录.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Phuan\Desktop\remote-repo\快递管理系统\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F368B73F-5581-405D-9791-C84FA7DD378C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B79305ED-89C0-47EE-A743-3662D11B934A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="21600" windowHeight="11295" xr2:uid="{067331B2-7E9C-4952-B8FB-432A4DD120A9}"/>
+    <workbookView xWindow="420" yWindow="-135" windowWidth="21600" windowHeight="11295" xr2:uid="{067331B2-7E9C-4952-B8FB-432A4DD120A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="58">
   <si>
     <t>项目信息</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -232,6 +232,56 @@
   </si>
   <si>
     <t>栅格系统的学习很大程度上解决了我在前几周作业中遇到的布局难的问题，简化了布局设计思路，并且成果布局更加稳定。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.10.09</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>① 经过在网络上查询，并且多次的自我尝试解决；
+② 仔细完成布置的SQL作业，在实践中提高自己对SQL的熟练度。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>①课程的第一部分首先对上次作业进行了讲评，展示了几位同学的前端设计成果，并将该前端作为本节课后端代码设计的基础。
+②进行了idea的后端环境配置，主要针对中文乱码的问题进行了讲解，经过多次尝试，最终解决了该问题。此外，编写了一段登陆用的后端代码，实现了前端到后端消息的简单传输。介绍了通过TOMCAT分别利用POST和GET两种信息传输方式的优缺点。
+③配置了数据库相关工具包——navicat和XAMPP，其中XAMPP内含mySQL、navicat可以实现对数据库的直观访问。利用navicat对SQL内容进行了复习，包括建表、基础增删改查、几种连接方式以及一些高级的查询写法。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>① IDEA中乱码问题的解决；
+② 对SQL遗忘较严重。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SQL语句的熟练使用是整个后端设计的重中之重，我会在课+A65:D68外的实践中不断提高自己SQL语句编写水平。此外我意识到，学习需要时刻对已学知识进行温习，温故而知新的道理在学习的路上长久适用。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2023.10.16</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>本堂课程延续上节课的内容，继续进行前后端的连接，首先回顾了上节课讲到的后端与前端连接的方法。本节课主要学习后端与数据库的连接方法，从JDBC、MVC模式以及ajax三部分进行学习。
+①JDBC相关内容。JDBC是最基础的数据库连接方式，首先进行了一系列驱动的加载，在后端代码中通过实现对数据库的增删改查的过程执行。
+②JavaWeb项目的MVC模式将项目分为三部分——分别是对象类、前端页面以及servlet。在数据库连接中，Model用于表示数据库中的数据结构和业务逻辑，View负责显示数据，Controller则负责接收用户请求、调用Model进行数据处理并更新View。
+③ajax在前后端交互中，可以允许在不重新加载页面的情况下，与后端服务器交换数据并更新网页内容。
+课程的后半部分针对之前的前端界面实现了登陆功能，包括从前端页面获取数据，通过ajax发送至后端服务器，利用JDBC对数据库进行增删改查操作，并将操作结果返回给后端服务器后发送至前端页面更新View。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>①第一次未顺利导入jar包
+②在进行数据库的增删改查操作时，sql语句逻辑处理中存在错误。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>①将数据库驱动jar包重新添加到正确路径得到解决。
+②需要继续熟悉SQL语句的使用。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>理论知识是基础，但只有通过实践才能真正掌握和运用。今天的课程中，我们通过真实的项目实践，对JDBC、MVC模式和ajax有了更深入的理解。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -355,6 +405,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -372,15 +431,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -705,10 +755,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C070542-4810-4C44-B3CA-BD4CD0234C21}">
-  <dimension ref="A1:E60"/>
+  <dimension ref="A1:E82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E57" sqref="E57"/>
+    <sheetView tabSelected="1" topLeftCell="A72" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A71" sqref="A71:D82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -720,12 +770,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="8"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="11"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -787,17 +837,17 @@
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="10"/>
-      <c r="D6" s="11"/>
+      <c r="C6" s="13"/>
+      <c r="D6" s="14"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="12"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="14"/>
+      <c r="A7" s="6"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="8"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
@@ -854,12 +904,12 @@
       <c r="D12" s="5"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="8"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="11"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
@@ -921,17 +971,17 @@
       <c r="A19" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="C19" s="10"/>
-      <c r="D19" s="11"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="14"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="12"/>
-      <c r="B20" s="13"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="14"/>
+      <c r="A20" s="6"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="8"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
@@ -988,12 +1038,12 @@
       <c r="D25" s="5"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" s="6" t="s">
+      <c r="A33" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B33" s="7"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="8"/>
+      <c r="B33" s="10"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="11"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
@@ -1055,17 +1105,17 @@
       <c r="A38" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B38" s="9" t="s">
+      <c r="B38" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="C38" s="10"/>
-      <c r="D38" s="11"/>
+      <c r="C38" s="13"/>
+      <c r="D38" s="14"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" s="12"/>
-      <c r="B39" s="13"/>
-      <c r="C39" s="13"/>
-      <c r="D39" s="14"/>
+      <c r="A39" s="6"/>
+      <c r="B39" s="7"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="8"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
@@ -1125,12 +1175,12 @@
       <c r="D44" s="5"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" s="6" t="s">
+      <c r="A49" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B49" s="7"/>
-      <c r="C49" s="7"/>
-      <c r="D49" s="8"/>
+      <c r="B49" s="10"/>
+      <c r="C49" s="10"/>
+      <c r="D49" s="11"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
@@ -1192,17 +1242,17 @@
       <c r="A54" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B54" s="9" t="s">
+      <c r="B54" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="C54" s="10"/>
-      <c r="D54" s="11"/>
+      <c r="C54" s="13"/>
+      <c r="D54" s="14"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55" s="12"/>
-      <c r="B55" s="13"/>
-      <c r="C55" s="13"/>
-      <c r="D55" s="14"/>
+      <c r="A55" s="6"/>
+      <c r="B55" s="7"/>
+      <c r="C55" s="7"/>
+      <c r="D55" s="8"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
@@ -1258,13 +1308,221 @@
       <c r="C60" s="4"/>
       <c r="D60" s="5"/>
     </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B64" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="176.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C65" s="4"/>
+      <c r="D65" s="5"/>
+    </row>
+    <row r="66" spans="1:4" ht="37.9" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C66" s="4"/>
+      <c r="D66" s="5"/>
+    </row>
+    <row r="67" spans="1:4" ht="52.15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C67" s="4"/>
+      <c r="D67" s="5"/>
+    </row>
+    <row r="68" spans="1:4" ht="69.599999999999994" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C68" s="4"/>
+      <c r="D68" s="5"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B71" s="10"/>
+      <c r="C71" s="10"/>
+      <c r="D71" s="11"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B72" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D73" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A74" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B74" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A75" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B75" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A76" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B76" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C76" s="13"/>
+      <c r="D76" s="14"/>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A77" s="6"/>
+      <c r="B77" s="7"/>
+      <c r="C77" s="7"/>
+      <c r="D77" s="8"/>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A78" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D78" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" ht="249.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A79" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C79" s="4"/>
+      <c r="D79" s="5"/>
+    </row>
+    <row r="80" spans="1:4" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A80" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C80" s="4"/>
+      <c r="D80" s="5"/>
+    </row>
+    <row r="81" spans="1:4" ht="39.6" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A81" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C81" s="4"/>
+      <c r="D81" s="5"/>
+    </row>
+    <row r="82" spans="1:4" ht="59.45" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A82" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C82" s="4"/>
+      <c r="D82" s="5"/>
+    </row>
   </sheetData>
-  <mergeCells count="28">
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="B12:D12"/>
+  <mergeCells count="39">
+    <mergeCell ref="B81:D81"/>
+    <mergeCell ref="B82:D82"/>
+    <mergeCell ref="A71:D71"/>
+    <mergeCell ref="B76:D76"/>
+    <mergeCell ref="A77:D77"/>
+    <mergeCell ref="B79:D79"/>
+    <mergeCell ref="B80:D80"/>
+    <mergeCell ref="B65:D65"/>
+    <mergeCell ref="B66:D66"/>
+    <mergeCell ref="B67:D67"/>
+    <mergeCell ref="B68:D68"/>
+    <mergeCell ref="B59:D59"/>
+    <mergeCell ref="B60:D60"/>
+    <mergeCell ref="A49:D49"/>
+    <mergeCell ref="B54:D54"/>
+    <mergeCell ref="A55:D55"/>
+    <mergeCell ref="B57:D57"/>
+    <mergeCell ref="B58:D58"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="A33:D33"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="A39:D39"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="B42:D42"/>
     <mergeCell ref="A7:D7"/>
     <mergeCell ref="A14:D14"/>
     <mergeCell ref="B19:D19"/>
@@ -1274,20 +1532,11 @@
     <mergeCell ref="B9:D9"/>
     <mergeCell ref="B10:D10"/>
     <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="A33:D33"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="A39:D39"/>
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="B42:D42"/>
-    <mergeCell ref="B59:D59"/>
-    <mergeCell ref="B60:D60"/>
-    <mergeCell ref="A49:D49"/>
-    <mergeCell ref="B54:D54"/>
-    <mergeCell ref="A55:D55"/>
-    <mergeCell ref="B57:D57"/>
-    <mergeCell ref="B58:D58"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B12:D12"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>